<commit_message>
update VehOutputAdap_SignalMatrix_V1_R2.xlsx update HkmcDiag arxml as R0 and add CddCanBusOff arxml update CddCanBusOff_SignalMatrix_V1_R1.xlsx
</commit_message>
<xml_diff>
--- a/R1/02_SignalMatrix/BSW/CddCanBusOff_SignalMatrix_V1_R1.xlsx
+++ b/R1/02_SignalMatrix/BSW/CddCanBusOff_SignalMatrix_V1_R1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasi.subrahmanyam\OneDrive - Veoneer\Documents\HKMC-Documents\CAN\R0\02_SignalMatrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R1\02_SignalMatrix\BSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{0E125839-809E-434B-AE31-E417D42DE756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{66ED8117-F345-482B-A286-1E825F68EB1B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A46D8-00E8-45BE-A60C-9C34AB6D99EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="22" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Change Log</t>
   </si>
@@ -139,9 +139,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>C/S</t>
-  </si>
-  <si>
     <t xml:space="preserve">From System Signal </t>
   </si>
   <si>
@@ -180,23 +177,31 @@
   <si>
     <t>CddCanBusOff ports</t>
   </si>
+  <si>
+    <t>Run_CddCanBusOff</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Client</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -207,7 +212,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -216,7 +221,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -224,20 +229,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -245,7 +250,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -253,7 +258,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -261,14 +266,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1125,16 +1130,16 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="72.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="72.625" customWidth="1"/>
+    <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" customHeight="1">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1167,7 +1172,7 @@
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
     </row>
-    <row r="2" spans="1:31" ht="15" thickBot="1">
+    <row r="2" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1200,7 +1205,7 @@
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="39" t="s">
         <v>0</v>
@@ -1235,7 +1240,7 @@
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
     </row>
-    <row r="4" spans="1:31" ht="15" thickBot="1">
+    <row r="4" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
@@ -1276,7 +1281,7 @@
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
     </row>
-    <row r="5" spans="1:31" ht="15" thickTop="1">
+    <row r="5" spans="1:31" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="9">
         <v>1</v>
@@ -1285,10 +1290,10 @@
         <v>44171</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="3"/>
@@ -1317,7 +1322,7 @@
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -1350,7 +1355,7 @@
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
@@ -1383,7 +1388,7 @@
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="9"/>
       <c r="C8" s="11"/>
@@ -1416,7 +1421,7 @@
       <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -1449,7 +1454,7 @@
       <c r="AD9" s="3"/>
       <c r="AE9" s="3"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="9"/>
       <c r="C10" s="11"/>
@@ -1482,7 +1487,7 @@
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
@@ -1515,7 +1520,7 @@
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="9"/>
       <c r="C12" s="11"/>
@@ -1548,7 +1553,7 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
     </row>
-    <row r="13" spans="1:31" ht="15" thickBot="1">
+    <row r="13" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1581,7 +1586,7 @@
       <c r="AD13" s="3"/>
       <c r="AE13" s="3"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1614,7 +1619,7 @@
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1647,7 +1652,7 @@
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1680,7 +1685,7 @@
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1713,7 +1718,7 @@
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1746,7 +1751,7 @@
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1779,7 +1784,7 @@
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1812,7 +1817,7 @@
       <c r="AD20" s="3"/>
       <c r="AE20" s="3"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1845,7 +1850,7 @@
       <c r="AD21" s="3"/>
       <c r="AE21" s="3"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1878,7 +1883,7 @@
       <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1911,7 +1916,7 @@
       <c r="AD23" s="3"/>
       <c r="AE23" s="3"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1944,7 +1949,7 @@
       <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1977,7 +1982,7 @@
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2010,7 +2015,7 @@
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2043,7 +2048,7 @@
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2076,7 +2081,7 @@
       <c r="AD28" s="3"/>
       <c r="AE28" s="3"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2109,7 +2114,7 @@
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2142,7 +2147,7 @@
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2175,7 +2180,7 @@
       <c r="AD31" s="3"/>
       <c r="AE31" s="3"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2208,7 +2213,7 @@
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2241,7 +2246,7 @@
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2274,7 +2279,7 @@
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2307,7 +2312,7 @@
       <c r="AD35" s="3"/>
       <c r="AE35" s="3"/>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2340,7 +2345,7 @@
       <c r="AD36" s="3"/>
       <c r="AE36" s="3"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2373,7 +2378,7 @@
       <c r="AD37" s="3"/>
       <c r="AE37" s="3"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2406,7 +2411,7 @@
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2439,7 +2444,7 @@
       <c r="AD39" s="3"/>
       <c r="AE39" s="3"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2472,7 +2477,7 @@
       <c r="AD40" s="3"/>
       <c r="AE40" s="3"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2505,7 +2510,7 @@
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2538,7 +2543,7 @@
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2571,7 +2576,7 @@
       <c r="AD43" s="3"/>
       <c r="AE43" s="3"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2604,7 +2609,7 @@
       <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2637,7 +2642,7 @@
       <c r="AD45" s="3"/>
       <c r="AE45" s="3"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2670,7 +2675,7 @@
       <c r="AD46" s="3"/>
       <c r="AE46" s="3"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2703,7 +2708,7 @@
       <c r="AD47" s="3"/>
       <c r="AE47" s="3"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2736,7 +2741,7 @@
       <c r="AD48" s="3"/>
       <c r="AE48" s="3"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -2764,7 +2769,7 @@
       <c r="AD49" s="3"/>
       <c r="AE49" s="3"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -2792,7 +2797,7 @@
       <c r="AD50" s="3"/>
       <c r="AE50" s="3"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -2838,34 +2843,34 @@
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R13" sqref="R13"/>
+      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="17.44140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="30.33203125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.44140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" style="29" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="17.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="30.375" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="29" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="30" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="6.625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" style="32" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.88671875" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" style="32" customWidth="1"/>
-    <col min="18" max="18" width="21.44140625" customWidth="1"/>
-    <col min="19" max="19" width="14.44140625" customWidth="1"/>
-    <col min="20" max="20" width="92.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.875" customWidth="1"/>
+    <col min="17" max="17" width="23.375" style="32" customWidth="1"/>
+    <col min="18" max="18" width="21.5" customWidth="1"/>
+    <col min="19" max="19" width="14.5" customWidth="1"/>
+    <col min="20" max="20" width="92.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="57.6">
+    <row r="1" spans="1:20" ht="66" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -2894,13 +2899,13 @@
         <v>5</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P1" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="37" t="s">
         <v>21</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>22</v>
       </c>
       <c r="R1" s="28" t="s">
         <v>10</v>
@@ -2912,37 +2917,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N2" s="34">
         <v>1</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R2" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S2" s="36" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="T2" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="O3"/>
       <c r="Q3"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="O5"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="O6"/>
     </row>
   </sheetData>
@@ -2960,27 +2965,27 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="35.625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" customWidth="1"/>
+    <col min="5" max="5" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
+    <col min="7" max="8" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
@@ -2991,14 +2996,14 @@
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="23"/>
@@ -3008,15 +3013,15 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>14</v>
@@ -3029,9 +3034,9 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3059,12 +3064,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3279,15 +3281,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b0add36e-da03-4abd-a3e0-9f2a80588293"/>
+    <ds:schemaRef ds:uri="ce510894-e256-4a70-bf8c-71462871c739"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3312,18 +3326,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b0add36e-da03-4abd-a3e0-9f2a80588293"/>
-    <ds:schemaRef ds:uri="ce510894-e256-4a70-bf8c-71462871c739"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>